<commit_message>
Ne plot x axis order
</commit_message>
<xml_diff>
--- a/analyses/Ne/NeEstimator/Correction/LinkageCorrection_cals.xlsx
+++ b/analyses/Ne/NeEstimator/Correction/LinkageCorrection_cals.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +573,10 @@
       <c r="H4" s="1">
         <v>190.7</v>
       </c>
+      <c r="J4" s="1">
+        <f>1/J2</f>
+        <v>1.274415842896927</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -622,6 +626,10 @@
       </c>
       <c r="H6" s="1">
         <v>1081.8</v>
+      </c>
+      <c r="J6" s="1">
+        <f>C5-C4</f>
+        <v>418.4</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -843,7 +851,7 @@
         <v>1374.2026033957563</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -875,7 +883,7 @@
         <v>3807.3173306545696</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -907,7 +915,7 @@
         <v>243.03110124044397</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
@@ -936,8 +944,12 @@
         <f t="shared" si="1"/>
         <v>930.19612373046698</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f>C19-C18</f>
+        <v>533.21558866807413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -969,7 +981,7 @@
         <v>1378.6630588458956</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>10</v>
@@ -999,7 +1011,7 @@
         <v>1440.5996688106864</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1031,7 +1043,7 @@
         <v>2640.3347433138538</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -1063,7 +1075,7 @@
         <v>1592.0002709468413</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1107,7 @@
         <v>533.34303025236397</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>1440.5996688106864</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1171,7 @@
         <v>2065.7006397516293</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1173,7 +1185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1199,7 @@
         <v>1202.2839061889608</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>